<commit_message>
Update tests to use ipachecklogic
</commit_message>
<xml_diff>
--- a/test/check06/check06_test01_in.xlsx
+++ b/test/check06/check06_test01_in.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\test\check06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherboyer/Dropbox/Github/scratch/high-frequency-checks/test/check06/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F748AD27-70D4-3045-9D98-3FD16F6BC960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" tabRatio="758" firstSheet="6" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17160" windowHeight="14440" tabRatio="758" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="3. consent" sheetId="3" r:id="rId4"/>
     <sheet name="4. no miss" sheetId="4" r:id="rId5"/>
     <sheet name="5. follow up" sheetId="5" r:id="rId6"/>
-    <sheet name="6. skip" sheetId="6" r:id="rId7"/>
+    <sheet name="6. logic" sheetId="6" r:id="rId7"/>
     <sheet name="7. all miss" sheetId="7" r:id="rId8"/>
     <sheet name="8. constraints" sheetId="8" r:id="rId9"/>
     <sheet name="9. specify" sheetId="9" r:id="rId10"/>
@@ -29,7 +30,7 @@
     <sheet name="research twoway" sheetId="17" r:id="rId15"/>
     <sheet name="researchdb" sheetId="14" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -210,8 +211,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -4618,7 +4619,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9820275" y="495300"/>
+          <a:off x="11176000" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -8345,7 +8346,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11391900" y="381000"/>
+          <a:off x="12966700" y="381000"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -10241,7 +10242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C33"/>
   <sheetViews>
@@ -10249,216 +10250,216 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="23" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1">
+    <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="11"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="11"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1">
+    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="11"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="11"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1">
+    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="11"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="11"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="11"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="11"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="11"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="11"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="11"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="11"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1">
+    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="22"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
     </row>
   </sheetData>
@@ -10471,7 +10472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -10479,9 +10480,9 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -10492,53 +10493,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" s="3"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" s="3"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C15" s="3"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C17" s="3"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
     </row>
@@ -10559,7 +10560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -10567,9 +10568,9 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -10592,19 +10593,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -10627,7 +10628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -10635,9 +10636,9 @@
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10652,19 +10653,19 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -10686,7 +10687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:F89"/>
   <sheetViews>
@@ -10694,9 +10695,9 @@
       <selection activeCell="A2" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -10716,13 +10717,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -10730,20 +10731,20 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -10751,11 +10752,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -10763,11 +10764,11 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -10775,11 +10776,11 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -10787,11 +10788,11 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -10799,11 +10800,11 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -10811,11 +10812,11 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -10823,11 +10824,11 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -10835,11 +10836,11 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -10847,11 +10848,11 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -10859,11 +10860,11 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -10871,11 +10872,11 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -10883,11 +10884,11 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -10895,11 +10896,11 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -10907,11 +10908,11 @@
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -10936,7 +10937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:C89"/>
   <sheetViews>
@@ -10944,9 +10945,9 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10957,155 +10958,155 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="C70" s="4"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="C81" s="4"/>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11127,17 +11128,17 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11151,149 +11152,149 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="4"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D37" s="4"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D59" s="4"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D70" s="4"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D81" s="4"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11316,7 +11317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -11324,9 +11325,9 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -11337,7 +11338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -11345,13 +11346,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11368,7 +11369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
@@ -11388,7 +11389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -11396,9 +11397,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11412,10 +11413,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
@@ -11435,7 +11436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -11443,9 +11444,9 @@
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11459,7 +11460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
@@ -11479,7 +11480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -11487,9 +11488,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11500,34 +11501,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
     </row>
   </sheetData>
@@ -11547,7 +11548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -11555,9 +11556,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11568,16 +11569,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
     </row>
   </sheetData>
@@ -11597,20 +11598,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -11641,18 +11642,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -11675,7 +11676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C602"/>
   <sheetViews>
@@ -11683,9 +11684,9 @@
       <selection activeCell="B32" sqref="B32:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11696,607 +11697,607 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C17" s="3"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C19" s="3"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" s="3"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C34" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C47" s="3"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C49" s="3"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C62" s="3"/>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C64" s="3"/>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77" s="3"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C79" s="3"/>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C92" s="3"/>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C94" s="3"/>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C107" s="3"/>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C109" s="3"/>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C122" s="3"/>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C124" s="3"/>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C137" s="3"/>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C139" s="3"/>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C152" s="3"/>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C154" s="3"/>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C167" s="3"/>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C169" s="3"/>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C182" s="3"/>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C184" s="3"/>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C197" s="3"/>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C199" s="3"/>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="3"/>
       <c r="B211" s="3"/>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C212" s="3"/>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C214" s="3"/>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="3"/>
       <c r="B226" s="3"/>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C227" s="3"/>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C229" s="3"/>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="3"/>
       <c r="B241" s="3"/>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C242" s="3"/>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C244" s="3"/>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="3"/>
       <c r="B255" s="3"/>
       <c r="C255" s="3"/>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="3"/>
       <c r="B256" s="3"/>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C257" s="3"/>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C259" s="3"/>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="3"/>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="3"/>
       <c r="B271" s="3"/>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C272" s="3"/>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C274" s="3"/>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="3"/>
       <c r="B285" s="3"/>
       <c r="C285" s="3"/>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="3"/>
       <c r="B286" s="3"/>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C287" s="3"/>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C289" s="3"/>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="3"/>
       <c r="B300" s="3"/>
       <c r="C300" s="3"/>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="3"/>
       <c r="B301" s="3"/>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C302" s="3"/>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C304" s="3"/>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="3"/>
       <c r="B315" s="3"/>
       <c r="C315" s="3"/>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="3"/>
       <c r="B316" s="3"/>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C317" s="3"/>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C319" s="3"/>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="3"/>
       <c r="B330" s="3"/>
       <c r="C330" s="3"/>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="3"/>
       <c r="B331" s="3"/>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C332" s="3"/>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C334" s="3"/>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" s="3"/>
       <c r="B345" s="3"/>
       <c r="C345" s="3"/>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" s="3"/>
       <c r="B346" s="3"/>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C347" s="3"/>
     </row>
-    <row r="349" spans="1:3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C349" s="3"/>
     </row>
-    <row r="360" spans="1:3">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="3"/>
       <c r="B360" s="3"/>
       <c r="C360" s="3"/>
     </row>
-    <row r="361" spans="1:3">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="3"/>
       <c r="B361" s="3"/>
     </row>
-    <row r="362" spans="1:3">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C362" s="3"/>
     </row>
-    <row r="364" spans="1:3">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C364" s="3"/>
     </row>
-    <row r="375" spans="1:3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="3"/>
       <c r="B375" s="3"/>
       <c r="C375" s="3"/>
     </row>
-    <row r="376" spans="1:3">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="3"/>
       <c r="B376" s="3"/>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C377" s="3"/>
     </row>
-    <row r="379" spans="1:3">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C379" s="3"/>
     </row>
-    <row r="390" spans="1:3">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390" s="3"/>
       <c r="B390" s="3"/>
       <c r="C390" s="3"/>
     </row>
-    <row r="391" spans="1:3">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391" s="3"/>
       <c r="B391" s="3"/>
     </row>
-    <row r="392" spans="1:3">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C392" s="3"/>
     </row>
-    <row r="394" spans="1:3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C394" s="3"/>
     </row>
-    <row r="405" spans="1:3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="3"/>
       <c r="B405" s="3"/>
       <c r="C405" s="3"/>
     </row>
-    <row r="406" spans="1:3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="3"/>
       <c r="B406" s="3"/>
     </row>
-    <row r="407" spans="1:3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C407" s="3"/>
     </row>
-    <row r="409" spans="1:3">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C409" s="3"/>
     </row>
-    <row r="420" spans="1:3">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="3"/>
       <c r="B420" s="3"/>
       <c r="C420" s="3"/>
     </row>
-    <row r="421" spans="1:3">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="3"/>
       <c r="B421" s="3"/>
     </row>
-    <row r="422" spans="1:3">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C422" s="3"/>
     </row>
-    <row r="424" spans="1:3">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C424" s="3"/>
     </row>
-    <row r="435" spans="1:3">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="3"/>
       <c r="B435" s="3"/>
       <c r="C435" s="3"/>
     </row>
-    <row r="436" spans="1:3">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="3"/>
       <c r="B436" s="3"/>
     </row>
-    <row r="437" spans="1:3">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C437" s="3"/>
     </row>
-    <row r="439" spans="1:3">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C439" s="3"/>
     </row>
-    <row r="450" spans="1:3">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A450" s="3"/>
       <c r="B450" s="3"/>
       <c r="C450" s="3"/>
     </row>
-    <row r="451" spans="1:3">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A451" s="3"/>
       <c r="B451" s="3"/>
     </row>
-    <row r="452" spans="1:3">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C452" s="3"/>
     </row>
-    <row r="454" spans="1:3">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C454" s="3"/>
     </row>
-    <row r="465" spans="1:3">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A465" s="3"/>
       <c r="B465" s="3"/>
       <c r="C465" s="3"/>
     </row>
-    <row r="466" spans="1:3">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A466" s="3"/>
       <c r="B466" s="3"/>
     </row>
-    <row r="467" spans="1:3">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C467" s="3"/>
     </row>
-    <row r="469" spans="1:3">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C469" s="3"/>
     </row>
-    <row r="480" spans="1:3">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A480" s="3"/>
       <c r="B480" s="3"/>
       <c r="C480" s="3"/>
     </row>
-    <row r="481" spans="1:3">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A481" s="3"/>
       <c r="B481" s="3"/>
     </row>
-    <row r="482" spans="1:3">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C482" s="3"/>
     </row>
-    <row r="484" spans="1:3">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C484" s="3"/>
     </row>
-    <row r="495" spans="1:3">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A495" s="3"/>
       <c r="B495" s="3"/>
       <c r="C495" s="3"/>
     </row>
-    <row r="496" spans="1:3">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A496" s="3"/>
       <c r="B496" s="3"/>
     </row>
-    <row r="497" spans="1:3">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C497" s="3"/>
     </row>
-    <row r="499" spans="1:3">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C499" s="3"/>
     </row>
-    <row r="510" spans="1:3">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A510" s="3"/>
       <c r="B510" s="3"/>
       <c r="C510" s="3"/>
     </row>
-    <row r="511" spans="1:3">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A511" s="3"/>
       <c r="B511" s="3"/>
     </row>
-    <row r="512" spans="1:3">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C512" s="3"/>
     </row>
-    <row r="514" spans="1:3">
+    <row r="514" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C514" s="3"/>
     </row>
-    <row r="525" spans="1:3">
+    <row r="525" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A525" s="3"/>
       <c r="B525" s="3"/>
       <c r="C525" s="3"/>
     </row>
-    <row r="526" spans="1:3">
+    <row r="526" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A526" s="3"/>
       <c r="B526" s="3"/>
     </row>
-    <row r="527" spans="1:3">
+    <row r="527" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C527" s="3"/>
     </row>
-    <row r="529" spans="1:3">
+    <row r="529" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C529" s="3"/>
     </row>
-    <row r="540" spans="1:3">
+    <row r="540" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A540" s="3"/>
       <c r="B540" s="3"/>
       <c r="C540" s="3"/>
     </row>
-    <row r="541" spans="1:3">
+    <row r="541" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A541" s="3"/>
       <c r="B541" s="3"/>
     </row>
-    <row r="542" spans="1:3">
+    <row r="542" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C542" s="3"/>
     </row>
-    <row r="544" spans="1:3">
+    <row r="544" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C544" s="3"/>
     </row>
-    <row r="555" spans="1:3">
+    <row r="555" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A555" s="3"/>
       <c r="B555" s="3"/>
       <c r="C555" s="3"/>
     </row>
-    <row r="556" spans="1:3">
+    <row r="556" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A556" s="3"/>
       <c r="B556" s="3"/>
     </row>
-    <row r="557" spans="1:3">
+    <row r="557" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C557" s="3"/>
     </row>
-    <row r="559" spans="1:3">
+    <row r="559" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C559" s="3"/>
     </row>
-    <row r="570" spans="1:3">
+    <row r="570" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A570" s="3"/>
       <c r="B570" s="3"/>
       <c r="C570" s="3"/>
     </row>
-    <row r="571" spans="1:3">
+    <row r="571" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A571" s="3"/>
       <c r="B571" s="3"/>
     </row>
-    <row r="572" spans="1:3">
+    <row r="572" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C572" s="3"/>
     </row>
-    <row r="574" spans="1:3">
+    <row r="574" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C574" s="3"/>
     </row>
-    <row r="585" spans="1:3">
+    <row r="585" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A585" s="3"/>
       <c r="B585" s="3"/>
       <c r="C585" s="3"/>
     </row>
-    <row r="586" spans="1:3">
+    <row r="586" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A586" s="3"/>
       <c r="B586" s="3"/>
     </row>
-    <row r="587" spans="1:3">
+    <row r="587" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C587" s="3"/>
     </row>
-    <row r="589" spans="1:3">
+    <row r="589" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C589" s="3"/>
     </row>
-    <row r="600" spans="1:3">
+    <row r="600" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A600" s="3"/>
       <c r="B600" s="3"/>
       <c r="C600" s="3"/>
     </row>
-    <row r="601" spans="1:3">
+    <row r="601" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A601" s="3"/>
       <c r="B601" s="3"/>
     </row>
-    <row r="602" spans="1:3">
+    <row r="602" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C602" s="3"/>
     </row>
   </sheetData>
@@ -12316,7 +12317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G72"/>
   <sheetViews>
@@ -12324,9 +12325,9 @@
       <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12349,465 +12350,465 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="2:6">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="2:6">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="2:6">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>

</xml_diff>